<commit_message>
Added Code to get the seasonal Data compared with Five Stations.
Added Code to get the seasonal Data compared with Five Stations.  Chart is a bit messed up. They are overlapping with each other. I will fix that later. I am tired. Must sleep. We made progress, good job. But I need to fix the seasonal chart again.
</commit_message>
<xml_diff>
--- a/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
+++ b/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
@@ -9,13 +9,16 @@
   <sheets>
     <sheet name="Ridership_2023" sheetId="1" r:id="rId1"/>
     <sheet name="Ridership_2024" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="Overall_Chart" sheetId="4" r:id="rId4"/>
+    <sheet name="Top_Stations_Chart" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="435">
   <si>
     <t>Station</t>
   </si>
@@ -1314,6 +1317,12 @@
   </si>
   <si>
     <t>Zerega Av (6)</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -1384,6 +1393,92 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>394357</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>45731</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="247650"/>
+          <a:ext cx="10881382" cy="5379731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>598578</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>83838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="247650"/>
+          <a:ext cx="13524003" cy="9037338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16279,4 +16374,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>273477612</v>
+      </c>
+      <c r="C2">
+        <v>290052145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>302476175</v>
+      </c>
+      <c r="C3">
+        <v>309827420</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>285632448</v>
+      </c>
+      <c r="C4">
+        <v>287299135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>302158187</v>
+      </c>
+      <c r="C5">
+        <v>324229714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="120.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="120.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Got the Bars between each season to be spaced out enough. Now I just need to..
Need to fix the spacing between each Station. It is too far apart. Also sometimes the number is so large that it gets cut off by the box line.  But then again, I am thinking about cutting this out. It may take too much time to get it right.
</commit_message>
<xml_diff>
--- a/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
+++ b/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
@@ -1449,9 +1449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>598578</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>83838</xdr:rowOff>
+      <xdr:colOff>568098</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>80808</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1469,7 +1469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="180975" y="247650"/>
-          <a:ext cx="13524003" cy="9037338"/>
+          <a:ext cx="13493523" cy="18178308"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Got Rid of the Gridlines and removed X axis Labels and numbers.
This makes it look much more better. Plus the numbers were a bit off. Next is to fix the other chart as well. Also made the box wider to let the numbers fit better.
</commit_message>
<xml_diff>
--- a/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
+++ b/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
@@ -1448,10 +1448,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>568098</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>290736</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>80808</xdr:rowOff>
+      <xdr:rowOff>99096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1469,7 +1469,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="180975" y="247650"/>
-          <a:ext cx="13493523" cy="18178308"/>
+          <a:ext cx="16264161" cy="18196596"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Updated Code to make the data into table format
Also removed the bad numbers from the charts as well.  Table is now color formatted.
</commit_message>
<xml_diff>
--- a/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
+++ b/Source/Data/Raw/Seasonal_Ridership_by_Station.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="436">
   <si>
     <t>Station</t>
   </si>
@@ -1323,6 +1323,9 @@
   </si>
   <si>
     <t>2024</t>
+  </si>
+  <si>
+    <t>Season</t>
   </si>
 </sst>
 </file>
@@ -1479,6 +1482,46 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E429" totalsRowShown="0">
+  <autoFilter ref="A1:E429"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Station"/>
+    <tableColumn id="2" name="Winter"/>
+    <tableColumn id="3" name="Spring"/>
+    <tableColumn id="4" name="Summer"/>
+    <tableColumn id="5" name="Fall"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E429" totalsRowShown="0">
+  <autoFilter ref="A1:E429"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Station"/>
+    <tableColumn id="2" name="Winter"/>
+    <tableColumn id="3" name="Spring"/>
+    <tableColumn id="4" name="Summer"/>
+    <tableColumn id="5" name="Fall"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Season"/>
+    <tableColumn id="2" name="2023"/>
+    <tableColumn id="3" name="2024"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1773,19 +1816,19 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -9067,6 +9110,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -9079,19 +9125,19 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -16373,6 +16419,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -16385,10 +16434,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" t="s">
         <v>433</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>434</v>
       </c>
     </row>
@@ -16438,6 +16490,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>